<commit_message>
First pass at providing PF for download via the GitBook.
</commit_message>
<xml_diff>
--- a/data/laminaria.xlsx
+++ b/data/laminaria.xlsx
@@ -118,6 +118,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -202,24 +203,23 @@
   <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.06632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>